<commit_message>
Refactor upload key handling in chat session and streamline startup script by removing unnecessary package installations
</commit_message>
<xml_diff>
--- a/sample_data/sadness_chat.xlsx
+++ b/sample_data/sadness_chat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\AI_Emotion_Management_Chatbot\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C265C943-05AA-4E63-A3BD-7D21D4F571FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16412814-6DAF-428A-961F-CD818B610870}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7935" xr2:uid="{2F85E0BD-4A1F-4DD7-A49F-7D71A263939A}"/>
   </bookViews>
@@ -25,39 +25,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>발신자,메시지,시간</t>
-  </si>
-  <si>
-    <t>A,"오늘 아침에 창밖을 보는데 비가 내리더라… 마음이 무거웠어",08:50</t>
   </si>
   <si>
     <t>B,"나도 창밖 보면서 괜히 쓸쓸해졌어",08:51</t>
   </si>
   <si>
-    <t>A,"출근길에 들었던 노래가 괜히 눈물이 나더라",09:10</t>
-  </si>
-  <si>
     <t>B,"그럴 때 있지… 가사 한 줄이 마음을 건드릴 때",09:11</t>
   </si>
   <si>
-    <t>A,"점심시간에 혼자 밥 먹으니까 더 외로웠어",12:20</t>
+    <t>A,"오늘 아침에 창밖을 보는데 비가 내리더라… 슬퍼졌어",08:50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>B,"나도 오늘은 같이 먹을 사람이 없어서 괜히 허전했어",12:21</t>
-  </si>
-  <si>
-    <t>A,"퇴근길에 불 꺼진 집에 들어가니까 공허하더라",18:40</t>
-  </si>
-  <si>
-    <t>B,"불 켜진 창문들 보면서 나만 혼자인 것 같은 기분 들 때 있지",18:41</t>
-  </si>
-  <si>
-    <t>A,"저녁 먹고도 마음이 가라앉아서 그냥 멍하니 있었어",20:10</t>
-  </si>
-  <si>
-    <t>B,"나도 그래… 오늘은 그냥 조용히 하루를 마무리하고 싶어",20:11</t>
+    <t>A,"출근길에 들었던 노래가 너무 슬프더라",09:10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -421,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8EDC4C-9FDE-4746-91E5-479E0972FD8C}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A6" sqref="A6:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -439,56 +423,27 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>